<commit_message>
1) Added camera controls by mouse click and drag. 2) Clean up the code.
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="14">
   <si>
     <t>Timestep</t>
   </si>
@@ -223,7 +223,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>48.0</v>
+        <v>5.0</v>
       </c>
       <c r="D4" t="n">
         <v>-320.67908473659566</v>

</xml_diff>

<commit_message>
1) Added initial pop up window to set initial conditions. 2) Fine tuned the camera angle. 3) Draw track selection.
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="14">
   <si>
     <t>Timestep</t>
   </si>
@@ -162,16 +162,16 @@
         <v>5.0</v>
       </c>
       <c r="I2" t="n">
-        <v>300.0</v>
+        <v>0.0</v>
       </c>
       <c r="J2" t="n">
         <v>0.0</v>
       </c>
       <c r="K2" t="n">
+        <v>-5.0</v>
+      </c>
+      <c r="L2" t="n">
         <v>0.0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>-5.0</v>
       </c>
       <c r="N2" t="n">
         <v>0.0</v>
@@ -187,73 +187,13 @@
       <c r="B3" t="n">
         <v>0.0</v>
       </c>
-      <c r="D3" t="n">
-        <v>-310.1931542970511</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-0.49559048973615366</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-0.02057113668330633</v>
-      </c>
-      <c r="G3" t="n">
-        <v>4.871405713675217</v>
-      </c>
-      <c r="I3" t="n">
-        <v>310.1931542970511</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.49559048973615366</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.02057113668330633</v>
-      </c>
-      <c r="L3" t="n">
-        <v>-4.871405713675217</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-74.87495948675371</v>
-      </c>
-      <c r="O3" t="n">
-        <v>2.6289706387185765</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-320.67908473659566</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-0.4601313348535672</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-0.017733285515600227</v>
-      </c>
-      <c r="G4" t="n">
-        <v>4.746197995759983</v>
-      </c>
-      <c r="I4" t="n">
-        <v>320.67908473659566</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.4601313348535672</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.017733285515600227</v>
-      </c>
-      <c r="L4" t="n">
-        <v>-4.746197995759983</v>
-      </c>
-      <c r="N4" t="n">
-        <v>-140.28355381364304</v>
-      </c>
-      <c r="O4" t="n">
-        <v>1.8262702819590102</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">

</xml_diff>